<commit_message>
Role classed added, now the full roleinfo will be parsed
</commit_message>
<xml_diff>
--- a/OpenWorld/Resources/Roles.xlsx
+++ b/OpenWorld/Resources/Roles.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8D0AA52-989F-44C5-8FD9-AF46DFC38E24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Warrior</t>
   </si>
@@ -35,12 +36,36 @@
   </si>
   <si>
     <t>name</t>
+  </si>
+  <si>
+    <t>hp increment</t>
+  </si>
+  <si>
+    <t>dmg increment</t>
+  </si>
+  <si>
+    <t>def increment</t>
+  </si>
+  <si>
+    <t>stamina increment</t>
+  </si>
+  <si>
+    <t>starting max hp</t>
+  </si>
+  <si>
+    <t>starting max dmg</t>
+  </si>
+  <si>
+    <t>starting def</t>
+  </si>
+  <si>
+    <t>starting max stamina</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -74,7 +99,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normál" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -90,7 +115,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-téma">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -165,6 +190,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -200,6 +242,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -375,48 +434,226 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
+      <c r="B2">
+        <v>12</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
+      <c r="B3">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>7</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>6</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>3</v>
+      </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
+      </c>
+      <c r="B7">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>10</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>3</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>